<commit_message>
Add JavaFaker for test data
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahobs\CIB_DigitalTech_UIAutomation\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -42,20 +43,43 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,8 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -376,7 +403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -384,7 +411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -392,12 +419,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Updated 'UpdatedDataInExcel' and changed Createdata method logic
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -3,21 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahobs\CIB_DigitalTech_UIAutomation\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760"/>
   </bookViews>
   <sheets>
-    <sheet name="UserDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="UserDetails" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,25 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Neo</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>firstName</t>
   </si>
@@ -61,12 +42,58 @@
   </si>
   <si>
     <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>uyuyu</t>
+  </si>
+  <si>
+    <t>yuyu</t>
+  </si>
+  <si>
+    <t>yuy</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Zulauf</t>
+  </si>
+  <si>
+    <t>up0t5s8v1</t>
+  </si>
+  <si>
+    <t>1-626-558-2900</t>
+  </si>
+  <si>
+    <t>CrystalZulauf35660</t>
+  </si>
+  <si>
+    <t>ignacio.bernhard@yahoo.com</t>
+  </si>
+  <si>
+    <t>Saul</t>
+  </si>
+  <si>
+    <t>Koch</t>
+  </si>
+  <si>
+    <t>6g4488swo2p5</t>
+  </si>
+  <si>
+    <t>250-664-9473</t>
+  </si>
+  <si>
+    <t>SaulKoch56660</t>
+  </si>
+  <si>
+    <t>drew.kiehn@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,86 +414,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Updated 'SelectDataInExcel' method with Apache POI implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>firstName</t>
   </si>
@@ -87,6 +87,42 @@
   </si>
   <si>
     <t>drew.kiehn@hotmail.com</t>
+  </si>
+  <si>
+    <t>Rupert</t>
+  </si>
+  <si>
+    <t>Kling</t>
+  </si>
+  <si>
+    <t>vlcwwpr64ji2fa</t>
+  </si>
+  <si>
+    <t>875-308-4141</t>
+  </si>
+  <si>
+    <t>RupertKling30576</t>
+  </si>
+  <si>
+    <t>yelena.abshire@hotmail.com</t>
+  </si>
+  <si>
+    <t>Ardath</t>
+  </si>
+  <si>
+    <t>Tromp</t>
+  </si>
+  <si>
+    <t>34mty8baa4yhl9n</t>
+  </si>
+  <si>
+    <t>1-398-863-1524</t>
+  </si>
+  <si>
+    <t>ArdathTromp01566</t>
+  </si>
+  <si>
+    <t>clayton.johnston@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -450,22 +486,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored reusable action methods
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="213">
   <si>
     <t>firstName</t>
   </si>
@@ -123,6 +123,546 @@
   </si>
   <si>
     <t>clayton.johnston@gmail.com</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Rosella</t>
+  </si>
+  <si>
+    <t>Nolan</t>
+  </si>
+  <si>
+    <t>885tsavx9</t>
+  </si>
+  <si>
+    <t>(926) 641-9324</t>
+  </si>
+  <si>
+    <t>RosellaNolan70749</t>
+  </si>
+  <si>
+    <t>grant.barton@gmail.com</t>
+  </si>
+  <si>
+    <t>Leigha</t>
+  </si>
+  <si>
+    <t>Pfeffer</t>
+  </si>
+  <si>
+    <t>wauwve3e34x</t>
+  </si>
+  <si>
+    <t>1-746-142-4100</t>
+  </si>
+  <si>
+    <t>LeighaPfeffer11349</t>
+  </si>
+  <si>
+    <t>emanuel.cartwright@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Batz</t>
+  </si>
+  <si>
+    <t>e1zanrh2a</t>
+  </si>
+  <si>
+    <t>198-307-1963</t>
+  </si>
+  <si>
+    <t>MikeBatz25975</t>
+  </si>
+  <si>
+    <t>jack.green@gmail.com</t>
+  </si>
+  <si>
+    <t>Cory</t>
+  </si>
+  <si>
+    <t>Collins</t>
+  </si>
+  <si>
+    <t>tdqt2qr6</t>
+  </si>
+  <si>
+    <t>(883) 446-8275</t>
+  </si>
+  <si>
+    <t>CoryCollins88571</t>
+  </si>
+  <si>
+    <t>rick.spinka@gmail.com</t>
+  </si>
+  <si>
+    <t>Stephani</t>
+  </si>
+  <si>
+    <t>Halvorson</t>
+  </si>
+  <si>
+    <t>bgnox0j76ukxpql</t>
+  </si>
+  <si>
+    <t>1-135-129-9750</t>
+  </si>
+  <si>
+    <t>StephaniHalvorson03225</t>
+  </si>
+  <si>
+    <t>betsey.armstrong@gmail.com</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Streich</t>
+  </si>
+  <si>
+    <t>17fbppnsigf3jg</t>
+  </si>
+  <si>
+    <t>333.485.2405</t>
+  </si>
+  <si>
+    <t>MorganStreich70104</t>
+  </si>
+  <si>
+    <t>annie.monahan@hotmail.com</t>
+  </si>
+  <si>
+    <t>Pinkie</t>
+  </si>
+  <si>
+    <t>Wolff</t>
+  </si>
+  <si>
+    <t>hg9uw7nreiw7nw</t>
+  </si>
+  <si>
+    <t>458.580.5201</t>
+  </si>
+  <si>
+    <t>PinkieWolff71147</t>
+  </si>
+  <si>
+    <t>minda.heidenreich@gmail.com</t>
+  </si>
+  <si>
+    <t>Valentine</t>
+  </si>
+  <si>
+    <t>Bruen</t>
+  </si>
+  <si>
+    <t>wwuixrnex</t>
+  </si>
+  <si>
+    <t>668-823-4531</t>
+  </si>
+  <si>
+    <t>ValentineBruen25049</t>
+  </si>
+  <si>
+    <t>quinn.oreilly@gmail.com</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Senger</t>
+  </si>
+  <si>
+    <t>cioqftaio5fqg</t>
+  </si>
+  <si>
+    <t>642.191.4119</t>
+  </si>
+  <si>
+    <t>MartinSenger88582</t>
+  </si>
+  <si>
+    <t>bernetta.hudson@hotmail.com</t>
+  </si>
+  <si>
+    <t>Ann</t>
+  </si>
+  <si>
+    <t>Hermiston</t>
+  </si>
+  <si>
+    <t>wri54hqm2</t>
+  </si>
+  <si>
+    <t>447.493.3422</t>
+  </si>
+  <si>
+    <t>AnnHermiston37826</t>
+  </si>
+  <si>
+    <t>elfreda.bashirian@gmail.com</t>
+  </si>
+  <si>
+    <t>Daryl</t>
+  </si>
+  <si>
+    <t>Daugherty</t>
+  </si>
+  <si>
+    <t>6glc7fvjb32z</t>
+  </si>
+  <si>
+    <t>1-168-376-5164</t>
+  </si>
+  <si>
+    <t>DarylDaugherty36540</t>
+  </si>
+  <si>
+    <t>ezra.pacocha@yahoo.com</t>
+  </si>
+  <si>
+    <t>Sha</t>
+  </si>
+  <si>
+    <t>Luettgen</t>
+  </si>
+  <si>
+    <t>03wm2zaa</t>
+  </si>
+  <si>
+    <t>(095) 095-0948</t>
+  </si>
+  <si>
+    <t>ShaLuettgen20506</t>
+  </si>
+  <si>
+    <t>sarah.corwin@hotmail.com</t>
+  </si>
+  <si>
+    <t>Horacio</t>
+  </si>
+  <si>
+    <t>Collier</t>
+  </si>
+  <si>
+    <t>x3zdnit5f7p</t>
+  </si>
+  <si>
+    <t>1-747-882-6582</t>
+  </si>
+  <si>
+    <t>HoracioCollier46676</t>
+  </si>
+  <si>
+    <t>todd.ortiz@yahoo.com</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Schuppe</t>
+  </si>
+  <si>
+    <t>jb9j50isk6hbxvd</t>
+  </si>
+  <si>
+    <t>615-325-5159</t>
+  </si>
+  <si>
+    <t>JeffSchuppe72913</t>
+  </si>
+  <si>
+    <t>dudley.langosh@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Wiza</t>
+  </si>
+  <si>
+    <t>idjiiu7en70</t>
+  </si>
+  <si>
+    <t>(269) 807-1570</t>
+  </si>
+  <si>
+    <t>MarkWiza71531</t>
+  </si>
+  <si>
+    <t>jann.auer@gmail.com</t>
+  </si>
+  <si>
+    <t>Kaycee</t>
+  </si>
+  <si>
+    <t>Wiegand</t>
+  </si>
+  <si>
+    <t>srk6nnuskntgz3</t>
+  </si>
+  <si>
+    <t>704-940-9497</t>
+  </si>
+  <si>
+    <t>KayceeWiegand05305</t>
+  </si>
+  <si>
+    <t>jefferson.mccullough@yahoo.com</t>
+  </si>
+  <si>
+    <t>Alyse</t>
+  </si>
+  <si>
+    <t>Runte</t>
+  </si>
+  <si>
+    <t>efoirzow</t>
+  </si>
+  <si>
+    <t>402-258-2795</t>
+  </si>
+  <si>
+    <t>AlyseRunte42246</t>
+  </si>
+  <si>
+    <t>rubie.kris@yahoo.com</t>
+  </si>
+  <si>
+    <t>Billy</t>
+  </si>
+  <si>
+    <t>Hessel</t>
+  </si>
+  <si>
+    <t>pgu774eyoni8</t>
+  </si>
+  <si>
+    <t>1-130-613-9741</t>
+  </si>
+  <si>
+    <t>BillyHessel85105</t>
+  </si>
+  <si>
+    <t>lionel.gusikowski@yahoo.com</t>
+  </si>
+  <si>
+    <t>Charise</t>
+  </si>
+  <si>
+    <t>Hudson</t>
+  </si>
+  <si>
+    <t>wnoejunm2aq6h5</t>
+  </si>
+  <si>
+    <t>655.100.2902</t>
+  </si>
+  <si>
+    <t>ChariseHudson10414</t>
+  </si>
+  <si>
+    <t>booker.dickinson@gmail.com</t>
+  </si>
+  <si>
+    <t>Drusilla</t>
+  </si>
+  <si>
+    <t>Willms</t>
+  </si>
+  <si>
+    <t>yqqw8ee23</t>
+  </si>
+  <si>
+    <t>(676) 744-3788</t>
+  </si>
+  <si>
+    <t>DrusillaWillms40880</t>
+  </si>
+  <si>
+    <t>velda.runolfsson@hotmail.com</t>
+  </si>
+  <si>
+    <t>Rayna</t>
+  </si>
+  <si>
+    <t>Huels</t>
+  </si>
+  <si>
+    <t>vca7zap75</t>
+  </si>
+  <si>
+    <t>(678) 855-8607</t>
+  </si>
+  <si>
+    <t>RaynaHuels86727</t>
+  </si>
+  <si>
+    <t>kenny.koch@yahoo.com</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Hickle</t>
+  </si>
+  <si>
+    <t>aow9vqfjnysx2</t>
+  </si>
+  <si>
+    <t>483-874-3439</t>
+  </si>
+  <si>
+    <t>SophiaHickle44027</t>
+  </si>
+  <si>
+    <t>robert.waelchi@gmail.com</t>
+  </si>
+  <si>
+    <t>Rosenda</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>miim6jpslbxfuog</t>
+  </si>
+  <si>
+    <t>921-524-2006</t>
+  </si>
+  <si>
+    <t>RosendaAdams28850</t>
+  </si>
+  <si>
+    <t>wilbur.bosco@gmail.com</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Abernathy</t>
+  </si>
+  <si>
+    <t>u6n1gxchhw3fsk</t>
+  </si>
+  <si>
+    <t>988-979-6798</t>
+  </si>
+  <si>
+    <t>JoeAbernathy88507</t>
+  </si>
+  <si>
+    <t>aron.dubuque@yahoo.com</t>
+  </si>
+  <si>
+    <t>Gail</t>
+  </si>
+  <si>
+    <t>Schulist</t>
+  </si>
+  <si>
+    <t>s9ymbsdy</t>
+  </si>
+  <si>
+    <t>1-992-301-5321</t>
+  </si>
+  <si>
+    <t>GailSchulist61436</t>
+  </si>
+  <si>
+    <t>elisha.weber@hotmail.com</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>7gzyrjdv3zr0w</t>
+  </si>
+  <si>
+    <t>571-624-0627</t>
+  </si>
+  <si>
+    <t>ChristopherWest27896</t>
+  </si>
+  <si>
+    <t>emerita.emmerich@gmail.com</t>
+  </si>
+  <si>
+    <t>Rochelle</t>
+  </si>
+  <si>
+    <t>Schaefer</t>
+  </si>
+  <si>
+    <t>cct63gr7yt70</t>
+  </si>
+  <si>
+    <t>491.374.7133</t>
+  </si>
+  <si>
+    <t>RochelleSchaefer37875</t>
+  </si>
+  <si>
+    <t>gussie.hintz@yahoo.com</t>
+  </si>
+  <si>
+    <t>Claudio</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>hn0tpx8ew6do</t>
+  </si>
+  <si>
+    <t>982.437.6624</t>
+  </si>
+  <si>
+    <t>ClaudioWalter16567</t>
+  </si>
+  <si>
+    <t>alberto.farrell@hotmail.com</t>
+  </si>
+  <si>
+    <t>Philip</t>
+  </si>
+  <si>
+    <t>Bergstrom</t>
+  </si>
+  <si>
+    <t>p8b2mnx4rwg7qwd</t>
+  </si>
+  <si>
+    <t>(045) 788-2719</t>
+  </si>
+  <si>
+    <t>PhilipBergstrom05350</t>
+  </si>
+  <si>
+    <t>hunter.rosenbaum@gmail.com</t>
+  </si>
+  <si>
+    <t>Elbert</t>
+  </si>
+  <si>
+    <t>tk3hr2ix</t>
+  </si>
+  <si>
+    <t>728.995.7008</t>
+  </si>
+  <si>
+    <t>ElbertLuettgen33325</t>
+  </si>
+  <si>
+    <t>glendora.ruecker@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -486,22 +1026,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>212</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Removed unused code
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="236">
   <si>
     <t>firstName</t>
   </si>
@@ -663,6 +663,75 @@
   </si>
   <si>
     <t>glendora.ruecker@gmail.com</t>
+  </si>
+  <si>
+    <t>Rocky</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>0mjompbhqt</t>
+  </si>
+  <si>
+    <t>011.028.0719</t>
+  </si>
+  <si>
+    <t>RockyRohan72449</t>
+  </si>
+  <si>
+    <t>renea.kulas@yahoo.com</t>
+  </si>
+  <si>
+    <t>Beulah</t>
+  </si>
+  <si>
+    <t>Treutel</t>
+  </si>
+  <si>
+    <t>j5h6djk8s</t>
+  </si>
+  <si>
+    <t>422.874.6791</t>
+  </si>
+  <si>
+    <t>BeulahTreutel06475</t>
+  </si>
+  <si>
+    <t>shantay.graham@gmail.com</t>
+  </si>
+  <si>
+    <t>Lexie</t>
+  </si>
+  <si>
+    <t>Altenwerth</t>
+  </si>
+  <si>
+    <t>bnovld5v9</t>
+  </si>
+  <si>
+    <t>1-376-864-1461</t>
+  </si>
+  <si>
+    <t>LexieAltenwerth60400</t>
+  </si>
+  <si>
+    <t>bradford.schowalter@yahoo.com</t>
+  </si>
+  <si>
+    <t>Hugh</t>
+  </si>
+  <si>
+    <t>lgojndxfu1tdpua</t>
+  </si>
+  <si>
+    <t>757-738-5941</t>
+  </si>
+  <si>
+    <t>HughRunte76417</t>
+  </si>
+  <si>
+    <t>josiah.watsica@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -1026,22 +1095,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="E2" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="F2" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Enhance reusability of code
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>FirstName</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Company BBB</t>
+  </si>
+  <si>
+    <t>0615186293</t>
+  </si>
+  <si>
+    <t>0479388126</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>6.651350157E9</v>
+        <v>2.521521663E9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -507,7 +513,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>6.651350157E9</v>
+        <v>2.521521663E9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
refactor: Enhance reusability of code and completed 'VerifyEntriesInTable' logic
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahobs\CIB_DigitalTech_UIAutomation\src\main\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahobs\Projects\Restore\CIB_DigitalTech-_UI\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -89,10 +89,22 @@
     <t>Company BBB</t>
   </si>
   <si>
-    <t>0615186293</t>
-  </si>
-  <si>
-    <t>0479388126</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>0713862369</t>
+  </si>
+  <si>
+    <t>0084824562</t>
+  </si>
+  <si>
+    <t>0393815750</t>
+  </si>
+  <si>
+    <t>0100118144</t>
+  </si>
+  <si>
+    <t>0128688953</t>
   </si>
 </sst>
 </file>
@@ -435,106 +447,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="20.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>2.521521663E9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2" t="n">
+        <v>1.216802002E9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>2.521521663E9</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="2" t="n">
+        <v>3.475716036E9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="mailto:admin@mail.com"/>
-    <hyperlink ref="G3" r:id="rId2" display="mailto:customer@mail.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="mailto:admin@mail.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="mailto:customer@mail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
refactor: further enhancement of 'VerifyEntriesInTable' logic
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>FirstName</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>0128688953</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1.216802002E9</v>
+        <v>5.697768474E9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -534,7 +537,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3.475716036E9</v>
+        <v>8.857887012E9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
refactor: Added additional test case as a result of a bug picked up and cleaned up the code
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>FirstName</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>0295788791</t>
+  </si>
+  <si>
+    <t>0116228842</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5.697768474E9</v>
+        <v>3.397453548E9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -537,7 +543,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>8.857887012E9</v>
+        <v>7.364775653E9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
add: Readme file and moved bug test to its own test class to demonstrate parallel execution.
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3.397453548E9</v>
+        <v>2.175983662E9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -543,7 +543,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>7.364775653E9</v>
+        <v>6.734743801E9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>

</xml_diff>